<commit_message>
Updates to fgoal preach configs
</commit_message>
<xml_diff>
--- a/experiments/results/initial/Aggregate Statistics.xlsx
+++ b/experiments/results/initial/Aggregate Statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e36e53eb9bd3f029/Thesis/ASH - Planner/experiments/results/initial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bham-my.sharepoint.com/personal/oxk312_student_bham_ac_uk/Documents/Desktop/ASH - Planner/experiments/results/initial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC104837291955FA5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18963882-D9A3-4C96-91EF-7958D22030FB}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="11_F25DC773A252ABDACC104837291955FA5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6549ACC6-1C30-482A-B20E-DAEAC2524C19}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="15030" yWindow="8540" windowWidth="17420" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Online" sheetId="1" r:id="rId1"/>
@@ -5392,7 +5392,7 @@
   <dimension ref="A1:Z119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF19" sqref="AF19"/>
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Cleaned up most results and logs.
</commit_message>
<xml_diff>
--- a/experiments/results/initial/Aggregate Statistics.xlsx
+++ b/experiments/results/initial/Aggregate Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bham-my.sharepoint.com/personal/oxk312_student_bham_ac_uk/Documents/Desktop/ASH - Planner/experiments/results/initial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e36e53eb9bd3f029/Desktop/ASH-Planner/experiments/results/initial/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="207" documentId="11_F25DC773A252ABDACC104837291955FA5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6549ACC6-1C30-482A-B20E-DAEAC2524C19}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15030" yWindow="8540" windowWidth="17420" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Online" sheetId="1" r:id="rId1"/>
@@ -4858,16 +4858,16 @@
             <v>4.324555467822172E-2</v>
           </cell>
           <cell r="L54">
-            <v>3.4260211949964557E-2</v>
+            <v>3.4260211949964564E-2</v>
           </cell>
           <cell r="M54">
             <v>5.834996447215153E-2</v>
           </cell>
           <cell r="N54">
-            <v>7.9947797581415639E-2</v>
+            <v>7.9947797581415403E-2</v>
           </cell>
           <cell r="O54">
-            <v>6.5392041961292557E-2</v>
+            <v>6.5392041961292544E-2</v>
           </cell>
           <cell r="P54">
             <v>0.10493093605563887</v>
@@ -5005,7 +5005,7 @@
             <v>1</v>
           </cell>
           <cell r="N57">
-            <v>0.55049197499386282</v>
+            <v>0.55049197499386293</v>
           </cell>
           <cell r="O57">
             <v>0.70077464242638188</v>
@@ -5046,7 +5046,7 @@
             <v>0.6829208263781259</v>
           </cell>
           <cell r="L58">
-            <v>0.84989496784968122</v>
+            <v>0.84989496784968133</v>
           </cell>
           <cell r="M58">
             <v>1</v>
@@ -5055,7 +5055,7 @@
             <v>0.62518650418588362</v>
           </cell>
           <cell r="O58">
-            <v>0.74718771150228414</v>
+            <v>0.74718771150228425</v>
           </cell>
           <cell r="P58">
             <v>0.9178082191780822</v>
@@ -5102,7 +5102,7 @@
             <v>0.66294053441504674</v>
           </cell>
           <cell r="O59">
-            <v>0.82203402544090443</v>
+            <v>0.82203402544090431</v>
           </cell>
           <cell r="P59">
             <v>0.95714285714285718</v>
@@ -5395,9 +5395,9 @@
       <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>[1]Globals!B52</f>
         <v>0</v>
@@ -5506,7 +5506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>[1]Globals!B53</f>
         <v>Mean</v>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>[1]Globals!B54</f>
         <v>Stdev</v>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>1.8416329928857361E-2</v>
+        <v>1.8416329928857365E-2</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>0.10575763587109316</v>
+        <v>0.10575763587109309</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
@@ -5701,14 +5701,14 @@
       </c>
       <c r="Y4">
         <f t="shared" ref="Y4:Y9" si="1">AVERAGE(V4:X4)</f>
-        <v>9.8779558268251286E-2</v>
+        <v>9.8779558268251258E-2</v>
       </c>
       <c r="Z4" t="b">
         <f>IF(Y4=MAX($Y$4,$Y$14,$Y$24,$Y$34),TRUE,FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>[1]Globals!B55</f>
         <v>Min</v>
@@ -5809,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>[1]Globals!B56</f>
         <v>LQ</v>
@@ -5910,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>[1]Globals!B57</f>
         <v>Med</v>
@@ -6011,7 +6011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>[1]Globals!B58</f>
         <v>UQ</v>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>0.81559178218736639</v>
+        <v>0.8155917821873665</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
@@ -6112,7 +6112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>[1]Globals!B59</f>
         <v>Max</v>
@@ -6213,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>[2]Globals!B52</f>
         <v>0</v>
@@ -6319,7 +6319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>[2]Globals!B53</f>
         <v>Mean</v>
@@ -6420,7 +6420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>[2]Globals!B54</f>
         <v>Stdev</v>
@@ -6521,7 +6521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>[2]Globals!B55</f>
         <v>Min</v>
@@ -6622,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>[2]Globals!B56</f>
         <v>LQ</v>
@@ -6723,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>[2]Globals!B57</f>
         <v>Med</v>
@@ -6824,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>[2]Globals!B58</f>
         <v>UQ</v>
@@ -6925,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>[2]Globals!B59</f>
         <v>Max</v>
@@ -7026,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>[3]Globals!B52</f>
         <v>0</v>
@@ -7132,7 +7132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>[3]Globals!B53</f>
         <v>Mean</v>
@@ -7233,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>[3]Globals!B54</f>
         <v>Stdev</v>
@@ -7334,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>[3]Globals!B55</f>
         <v>Min</v>
@@ -7435,7 +7435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>[3]Globals!B56</f>
         <v>LQ</v>
@@ -7536,7 +7536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>[3]Globals!B57</f>
         <v>Med</v>
@@ -7637,7 +7637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>[3]Globals!B58</f>
         <v>UQ</v>
@@ -7738,7 +7738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>[3]Globals!B59</f>
         <v>Max</v>
@@ -7839,7 +7839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>[4]Globals!B52</f>
         <v>0</v>
@@ -7945,7 +7945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>[4]Globals!B53</f>
         <v>Mean</v>
@@ -8046,7 +8046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>[4]Globals!B54</f>
         <v>Stdev</v>
@@ -8147,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>[4]Globals!B55</f>
         <v>Min</v>
@@ -8248,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>[4]Globals!B56</f>
         <v>LQ</v>
@@ -8349,7 +8349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>[4]Globals!B57</f>
         <v>Med</v>
@@ -8450,7 +8450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>[4]Globals!B58</f>
         <v>UQ</v>
@@ -8551,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>[4]Globals!B59</f>
         <v>Max</v>
@@ -8652,7 +8652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>[5]Globals!B52</f>
         <v>0</v>
@@ -8725,7 +8725,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>[5]Globals!B53</f>
         <v>Mean</v>
@@ -8787,7 +8787,7 @@
         <v>0.81246265741239165</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>[5]Globals!B54</f>
         <v>Stdev</v>
@@ -8849,7 +8849,7 @@
         <v>8.6642406566445923E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>[5]Globals!B55</f>
         <v>Min</v>
@@ -8911,7 +8911,7 @@
         <v>0.68831168831168832</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>[5]Globals!B56</f>
         <v>LQ</v>
@@ -8973,7 +8973,7 @@
         <v>0.72602739726027399</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>[5]Globals!B57</f>
         <v>Med</v>
@@ -9035,7 +9035,7 @@
         <v>0.77958035907419421</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>[5]Globals!B58</f>
         <v>UQ</v>
@@ -9097,7 +9097,7 @@
         <v>0.89830508474576276</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>[5]Globals!B59</f>
         <v>Max</v>
@@ -9159,7 +9159,7 @@
         <v>0.96363636363636362</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>[6]Globals!B52</f>
         <v>0</v>
@@ -9232,7 +9232,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>[6]Globals!B53</f>
         <v>Mean</v>
@@ -9294,7 +9294,7 @@
         <v>0.80991156501196626</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>[6]Globals!B54</f>
         <v>Stdev</v>
@@ -9356,7 +9356,7 @@
         <v>9.8573841322420544E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>[6]Globals!B55</f>
         <v>Min</v>
@@ -9418,7 +9418,7 @@
         <v>0.67088607594936711</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>[6]Globals!B56</f>
         <v>LQ</v>
@@ -9480,7 +9480,7 @@
         <v>0.72602739726027399</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>[6]Globals!B57</f>
         <v>Med</v>
@@ -9542,7 +9542,7 @@
         <v>0.80303030303030298</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>[6]Globals!B58</f>
         <v>UQ</v>
@@ -9604,7 +9604,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>[6]Globals!B59</f>
         <v>Max</v>
@@ -9666,7 +9666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>[7]Globals!B52</f>
         <v>0</v>
@@ -9739,7 +9739,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>[7]Globals!B53</f>
         <v>Mean</v>
@@ -9801,7 +9801,7 @@
         <v>0.76479077199277257</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>[7]Globals!B54</f>
         <v>Stdev</v>
@@ -9863,7 +9863,7 @@
         <v>8.4318306335268198E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>[7]Globals!B55</f>
         <v>Min</v>
@@ -9925,7 +9925,7 @@
         <v>0.70666666666666667</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>[7]Globals!B56</f>
         <v>LQ</v>
@@ -9987,7 +9987,7 @@
         <v>0.70666666666666667</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>[7]Globals!B57</f>
         <v>Med</v>
@@ -10049,7 +10049,7 @@
         <v>0.72602739726027399</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>[7]Globals!B58</f>
         <v>UQ</v>
@@ -10111,7 +10111,7 @@
         <v>0.79104477611940294</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>[7]Globals!B59</f>
         <v>Max</v>
@@ -10173,7 +10173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>[8]Globals!B52</f>
         <v>0</v>
@@ -10246,7 +10246,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>[8]Globals!B53</f>
         <v>Mean</v>
@@ -10308,7 +10308,7 @@
         <v>0.77452102910279952</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>[8]Globals!B54</f>
         <v>Stdev</v>
@@ -10370,7 +10370,7 @@
         <v>9.0813546332030134E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>[8]Globals!B55</f>
         <v>Min</v>
@@ -10432,7 +10432,7 @@
         <v>0.66249999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>[8]Globals!B56</f>
         <v>LQ</v>
@@ -10494,7 +10494,7 @@
         <v>0.67948717948717952</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>[8]Globals!B57</f>
         <v>Med</v>
@@ -10556,7 +10556,7 @@
         <v>0.76811594202898548</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>[8]Globals!B58</f>
         <v>UQ</v>
@@ -10618,7 +10618,7 @@
         <v>0.87757496740547591</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>[8]Globals!B59</f>
         <v>Max</v>
@@ -10680,7 +10680,7 @@
         <v>0.92982456140350878</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>[9]Globals!B52</f>
         <v>0</v>
@@ -10753,7 +10753,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>[9]Globals!B53</f>
         <v>Mean</v>
@@ -10815,7 +10815,7 @@
         <v>0.82289568297956972</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>[9]Globals!B54</f>
         <v>Stdev</v>
@@ -10858,7 +10858,7 @@
       </c>
       <c r="K84">
         <f>[9]Globals!L54</f>
-        <v>3.4260211949964557E-2</v>
+        <v>3.4260211949964564E-2</v>
       </c>
       <c r="L84">
         <f>[9]Globals!M54</f>
@@ -10866,18 +10866,18 @@
       </c>
       <c r="M84">
         <f>[9]Globals!N54</f>
-        <v>7.9947797581415639E-2</v>
+        <v>7.9947797581415403E-2</v>
       </c>
       <c r="N84">
         <f>[9]Globals!O54</f>
-        <v>6.5392041961292557E-2</v>
+        <v>6.5392041961292544E-2</v>
       </c>
       <c r="O84">
         <f>[9]Globals!P54</f>
         <v>0.10493093605563887</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>[9]Globals!B55</f>
         <v>Min</v>
@@ -10939,7 +10939,7 @@
         <v>0.53208978821536002</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>[9]Globals!B56</f>
         <v>LQ</v>
@@ -11001,7 +11001,7 @@
         <v>0.77235364875701684</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>[9]Globals!B57</f>
         <v>Med</v>
@@ -11052,7 +11052,7 @@
       </c>
       <c r="M87">
         <f>[9]Globals!N57</f>
-        <v>0.55049197499386282</v>
+        <v>0.55049197499386293</v>
       </c>
       <c r="N87">
         <f>[9]Globals!O57</f>
@@ -11063,7 +11063,7 @@
         <v>0.81719470474490552</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>[9]Globals!B58</f>
         <v>UQ</v>
@@ -11106,7 +11106,7 @@
       </c>
       <c r="K88">
         <f>[9]Globals!L58</f>
-        <v>0.84989496784968122</v>
+        <v>0.84989496784968133</v>
       </c>
       <c r="L88">
         <f>[9]Globals!M58</f>
@@ -11118,14 +11118,14 @@
       </c>
       <c r="N88">
         <f>[9]Globals!O58</f>
-        <v>0.74718771150228414</v>
+        <v>0.74718771150228425</v>
       </c>
       <c r="O88">
         <f>[9]Globals!P58</f>
         <v>0.9178082191780822</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>[9]Globals!B59</f>
         <v>Max</v>
@@ -11180,14 +11180,14 @@
       </c>
       <c r="N89">
         <f>[9]Globals!O59</f>
-        <v>0.82203402544090443</v>
+        <v>0.82203402544090431</v>
       </c>
       <c r="O89">
         <f>[9]Globals!P59</f>
         <v>0.95714285714285718</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92">
         <f>[10]Globals!B52</f>
         <v>0</v>
@@ -11260,7 +11260,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>[10]Globals!B53</f>
         <v>Mean</v>
@@ -11322,7 +11322,7 @@
         <v>0.80532483496000429</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>[10]Globals!B54</f>
         <v>Stdev</v>
@@ -11384,7 +11384,7 @@
         <v>8.2594686604439527E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>[10]Globals!B55</f>
         <v>Min</v>
@@ -11446,7 +11446,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>[10]Globals!B56</f>
         <v>LQ</v>
@@ -11508,7 +11508,7 @@
         <v>0.73830891330891335</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>[10]Globals!B57</f>
         <v>Med</v>
@@ -11570,7 +11570,7 @@
         <v>0.78823529411764703</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>[10]Globals!B58</f>
         <v>UQ</v>
@@ -11632,7 +11632,7 @@
         <v>0.84545094936708853</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>[10]Globals!B59</f>
         <v>Max</v>
@@ -11694,7 +11694,7 @@
         <v>0.97101449275362317</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>19</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>[11]Globals!B52</f>
         <v>0</v>
@@ -11767,7 +11767,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>[11]Globals!B53</f>
         <v>Mean</v>
@@ -11829,7 +11829,7 @@
         <v>0.83149302888349408</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>[11]Globals!B54</f>
         <v>Stdev</v>
@@ -11891,7 +11891,7 @@
         <v>7.3229435634959053E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>[11]Globals!B55</f>
         <v>Min</v>
@@ -11953,7 +11953,7 @@
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>[11]Globals!B56</f>
         <v>LQ</v>
@@ -12015,7 +12015,7 @@
         <v>0.78823529411764703</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>[11]Globals!B57</f>
         <v>Med</v>
@@ -12077,7 +12077,7 @@
         <v>0.81707317073170727</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>[11]Globals!B58</f>
         <v>UQ</v>
@@ -12139,7 +12139,7 @@
         <v>0.911689497716895</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>[11]Globals!B59</f>
         <v>Max</v>
@@ -12201,7 +12201,7 @@
         <v>0.94366197183098588</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>19</v>
       </c>
@@ -12212,7 +12212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112">
         <f>[12]Globals!B52</f>
         <v>0</v>
@@ -12274,7 +12274,7 @@
         <v>WT</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>[12]Globals!B53</f>
         <v>Mean</v>
@@ -12336,7 +12336,7 @@
         <v>0.77767796129395361</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>[12]Globals!B54</f>
         <v>Stdev</v>
@@ -12398,7 +12398,7 @@
         <v>7.8006721312238403E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>[12]Globals!B55</f>
         <v>Min</v>
@@ -12460,7 +12460,7 @@
         <v>0.6633663366336634</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f>[12]Globals!B56</f>
         <v>LQ</v>
@@ -12522,7 +12522,7 @@
         <v>0.71663968547641077</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f>[12]Globals!B57</f>
         <v>Med</v>
@@ -12584,7 +12584,7 @@
         <v>0.77011494252873558</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f>[12]Globals!B58</f>
         <v>UQ</v>
@@ -12646,7 +12646,7 @@
         <v>0.81977513227513232</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f>[12]Globals!B59</f>
         <v>Max</v>

</xml_diff>